<commit_message>
alembic: add data table citys
</commit_message>
<xml_diff>
--- a/data/city.xlsx
+++ b/data/city.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Мой диск\Проекты\AirportDirectory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\AirportDirectory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7BBA3F-C0F8-4653-BB3F-C46E54684E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F0A345-483F-409E-9926-21205D87A733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="9432" xr2:uid="{711EE758-C8BF-442E-9FC3-C85971365277}"/>
   </bookViews>
@@ -2127,7 +2127,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
data: sorted by city
</commit_message>
<xml_diff>
--- a/data/city.xlsx
+++ b/data/city.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\AirportDirectory\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F0A345-483F-409E-9926-21205D87A733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E967D7A0-8CFB-408F-999A-D563723822A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="9432" xr2:uid="{711EE758-C8BF-442E-9FC3-C85971365277}"/>
   </bookViews>
@@ -2127,7 +2127,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2154,16 +2154,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>378</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>379</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>380</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2171,1483 +2171,1483 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>409</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>411</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>298</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>299</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>409</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>72</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>410</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>406</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>407</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>408</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>397</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>399</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>188</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>34</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>359</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>360</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>361</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>345</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>349</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>350</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>406</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>407</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>408</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>333</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>334</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>335</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>65</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>382</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>383</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>384</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>69</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>320</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>321</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>374</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>375</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>376</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>92</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>352</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>353</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>354</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>367</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>368</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>369</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>104</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>316</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>323</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>324</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>117</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>128</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>132</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>20</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>144</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B43" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>304</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>305</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>306</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>161</v>
+        <v>307</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>317</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>318</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>164</v>
+        <v>319</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>165</v>
+        <v>252</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>256</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>257</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>168</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="B49" t="s">
-        <v>170</v>
+        <v>403</v>
       </c>
       <c r="C49" t="s">
-        <v>171</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>172</v>
+        <v>404</v>
+      </c>
+      <c r="D49" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>177</v>
+        <v>367</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>371</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>372</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>180</v>
+        <v>373</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>403</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
-        <v>404</v>
-      </c>
-      <c r="D52" t="s">
-        <v>405</v>
+        <v>116</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>329</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>330</v>
       </c>
       <c r="C53" t="s">
-        <v>184</v>
+        <v>331</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>185</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>187</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>188</v>
+        <v>68</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>189</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>192</v>
+        <v>30</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>193</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>390</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>391</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
+        <v>392</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>197</v>
+        <v>393</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>199</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>200</v>
+        <v>103</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>201</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="C58" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>206</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>207</v>
+        <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C60" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
       <c r="B61" t="s">
-        <v>213</v>
+        <v>282</v>
       </c>
       <c r="C61" t="s">
-        <v>214</v>
+        <v>283</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>215</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>218</v>
+        <v>23</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>219</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C63" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C64" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="C65" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B66" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
-        <v>232</v>
+        <v>7</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>233</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="C67" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>237</v>
+        <v>341</v>
       </c>
       <c r="B68" t="s">
-        <v>238</v>
+        <v>342</v>
       </c>
       <c r="C68" t="s">
-        <v>239</v>
+        <v>343</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>240</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>241</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>242</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>243</v>
+        <v>131</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>244</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="C70" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>248</v>
+        <v>35</v>
       </c>
       <c r="B71" t="s">
-        <v>249</v>
+        <v>45</v>
       </c>
       <c r="C71" t="s">
-        <v>250</v>
+        <v>46</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>251</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="B72" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="C72" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>252</v>
+        <v>226</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="C73" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>258</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B74" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="C74" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>263</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
-        <v>264</v>
+        <v>159</v>
       </c>
       <c r="C75" t="s">
-        <v>265</v>
+        <v>160</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>266</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>267</v>
+        <v>355</v>
       </c>
       <c r="B76" t="s">
-        <v>268</v>
+        <v>356</v>
       </c>
       <c r="C76" t="s">
-        <v>269</v>
+        <v>357</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>270</v>
+        <v>358</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="B77" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
       <c r="C77" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>271</v>
+        <v>59</v>
       </c>
       <c r="B78" t="s">
-        <v>275</v>
+        <v>63</v>
       </c>
       <c r="C78" t="s">
-        <v>276</v>
+        <v>64</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>277</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>278</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>279</v>
+        <v>146</v>
       </c>
       <c r="C79" t="s">
-        <v>280</v>
+        <v>147</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>281</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
       <c r="B80" t="s">
-        <v>282</v>
+        <v>249</v>
       </c>
       <c r="C80" t="s">
-        <v>283</v>
+        <v>250</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>285</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>286</v>
+        <v>15</v>
       </c>
       <c r="C81" t="s">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>288</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>289</v>
+        <v>35</v>
       </c>
       <c r="B82" t="s">
-        <v>290</v>
+        <v>36</v>
       </c>
       <c r="C82" t="s">
-        <v>291</v>
+        <v>37</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>292</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>293</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>294</v>
+        <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>295</v>
+        <v>79</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>296</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>297</v>
+        <v>271</v>
       </c>
       <c r="B84" t="s">
-        <v>298</v>
+        <v>275</v>
       </c>
       <c r="C84" t="s">
-        <v>299</v>
+        <v>276</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>300</v>
+        <v>277</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>301</v>
+        <v>345</v>
       </c>
       <c r="B85" t="s">
-        <v>302</v>
+        <v>346</v>
       </c>
       <c r="C85" t="s">
-        <v>303</v>
+        <v>347</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>96</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>304</v>
+        <v>216</v>
       </c>
       <c r="B86" t="s">
-        <v>305</v>
+        <v>220</v>
       </c>
       <c r="C86" t="s">
-        <v>306</v>
+        <v>221</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>307</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>308</v>
+        <v>252</v>
       </c>
       <c r="B87" t="s">
-        <v>309</v>
+        <v>253</v>
       </c>
       <c r="C87" t="s">
-        <v>310</v>
+        <v>254</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>311</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>312</v>
+        <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>313</v>
+        <v>122</v>
       </c>
       <c r="C88" t="s">
-        <v>314</v>
+        <v>123</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>315</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>316</v>
+        <v>158</v>
       </c>
       <c r="B89" t="s">
-        <v>317</v>
+        <v>162</v>
       </c>
       <c r="C89" t="s">
-        <v>318</v>
+        <v>163</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>319</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>316</v>
+        <v>259</v>
       </c>
       <c r="B90" t="s">
-        <v>320</v>
+        <v>260</v>
       </c>
       <c r="C90" t="s">
-        <v>321</v>
+        <v>261</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>322</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>316</v>
+        <v>263</v>
       </c>
       <c r="B91" t="s">
-        <v>323</v>
+        <v>264</v>
       </c>
       <c r="C91" t="s">
-        <v>324</v>
+        <v>265</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>325</v>
+        <v>266</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>316</v>
+        <v>267</v>
       </c>
       <c r="B92" t="s">
-        <v>326</v>
+        <v>268</v>
       </c>
       <c r="C92" t="s">
-        <v>327</v>
+        <v>269</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>328</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="B93" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="C93" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="B94" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="C94" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>337</v>
+        <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>338</v>
+        <v>32</v>
       </c>
       <c r="C95" t="s">
-        <v>339</v>
+        <v>33</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>340</v>
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>341</v>
+        <v>308</v>
       </c>
       <c r="B96" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="C96" t="s">
-        <v>343</v>
+        <v>310</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>344</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>345</v>
+        <v>145</v>
       </c>
       <c r="B97" t="s">
-        <v>346</v>
+        <v>152</v>
       </c>
       <c r="C97" t="s">
-        <v>347</v>
+        <v>153</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>348</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>345</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>349</v>
+        <v>49</v>
       </c>
       <c r="C98" t="s">
-        <v>350</v>
+        <v>50</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>351</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>352</v>
+        <v>271</v>
       </c>
       <c r="B99" t="s">
-        <v>353</v>
+        <v>272</v>
       </c>
       <c r="C99" t="s">
-        <v>354</v>
+        <v>273</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>6</v>
+        <v>274</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>355</v>
+        <v>316</v>
       </c>
       <c r="B100" t="s">
-        <v>356</v>
+        <v>326</v>
       </c>
       <c r="C100" t="s">
-        <v>357</v>
+        <v>327</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>358</v>
+        <v>328</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>359</v>
+        <v>386</v>
       </c>
       <c r="B101" t="s">
-        <v>360</v>
+        <v>387</v>
       </c>
       <c r="C101" t="s">
-        <v>361</v>
+        <v>388</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>362</v>
+        <v>389</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>363</v>
+        <v>289</v>
       </c>
       <c r="B102" t="s">
-        <v>364</v>
+        <v>290</v>
       </c>
       <c r="C102" t="s">
-        <v>365</v>
+        <v>291</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>366</v>
+        <v>292</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B103" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C103" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>367</v>
+        <v>293</v>
       </c>
       <c r="B104" t="s">
-        <v>371</v>
+        <v>294</v>
       </c>
       <c r="C104" t="s">
-        <v>372</v>
+        <v>295</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>373</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>374</v>
+        <v>216</v>
       </c>
       <c r="B105" t="s">
-        <v>375</v>
+        <v>223</v>
       </c>
       <c r="C105" t="s">
-        <v>376</v>
+        <v>224</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>377</v>
+        <v>225</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>378</v>
+        <v>337</v>
       </c>
       <c r="B106" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="C106" t="s">
-        <v>380</v>
+        <v>339</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>381</v>
+        <v>340</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>382</v>
+        <v>230</v>
       </c>
       <c r="B107" t="s">
-        <v>383</v>
+        <v>231</v>
       </c>
       <c r="C107" t="s">
-        <v>384</v>
+        <v>232</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>385</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>386</v>
+        <v>237</v>
       </c>
       <c r="B108" t="s">
-        <v>387</v>
+        <v>238</v>
       </c>
       <c r="C108" t="s">
-        <v>388</v>
+        <v>239</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>389</v>
+        <v>240</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -3655,41 +3655,41 @@
         <v>390</v>
       </c>
       <c r="B109" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C109" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>390</v>
+        <v>145</v>
       </c>
       <c r="B110" t="s">
-        <v>394</v>
+        <v>155</v>
       </c>
       <c r="C110" t="s">
-        <v>395</v>
+        <v>156</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>396</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>397</v>
+        <v>301</v>
       </c>
       <c r="B111" t="s">
-        <v>398</v>
+        <v>302</v>
       </c>
       <c r="C111" t="s">
-        <v>399</v>
+        <v>303</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>400</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -15414,6 +15414,9 @@
       <c r="D4018"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D111">
+    <sortCondition ref="B2:B111"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>